<commit_message>
chore:L fixed variable names
</commit_message>
<xml_diff>
--- a/dictionaries/methylclocks/mc-yearly-rep.xlsx
+++ b/dictionaries/methylclocks/mc-yearly-rep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_clocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylclocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F509FA1-A97A-C04D-89FE-1CB85CECB2B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723BE749-7EA4-1D49-93E5-E82FF1BDF36B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="500" windowWidth="15960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="88040" yWindow="500" windowWidth="15960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>Age 3 for PedBE measurement</t>
+  </si>
+  <si>
+    <t>ageAcc2.PedBE</t>
+  </si>
+  <si>
+    <t>ageAcc3.PedBE</t>
+  </si>
+  <si>
+    <t>ageAcc2.skinHorvath</t>
+  </si>
+  <si>
+    <t>ageAcc3.skinHorvath</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1444,7 @@
   <dimension ref="A1:IP31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5169,7 +5181,7 @@
     </row>
     <row r="21" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>9</v>
@@ -5429,7 +5441,7 @@
     </row>
     <row r="22" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>9</v>
@@ -5963,7 +5975,7 @@
     </row>
     <row r="25" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>9</v>
@@ -6223,7 +6235,7 @@
     </row>
     <row r="26" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add TL and age variables
</commit_message>
<xml_diff>
--- a/dictionaries/methylclocks/mc-yearly-rep.xlsx
+++ b/dictionaries/methylclocks/mc-yearly-rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylclocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justiina\Desktop\DNAm age\Methylclock\datashield\ds-beta-dictionaries\dictionaries\methylclocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723BE749-7EA4-1D49-93E5-E82FF1BDF36B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E95DCB-2F10-4BA7-811B-54D3901085FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="88040" yWindow="500" windowWidth="15960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -187,12 +187,24 @@
   <si>
     <t>ageAcc3.skinHorvath</t>
   </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Chronological age</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Telomere length estimate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -257,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -269,6 +281,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1441,21 +1454,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP31"/>
+  <dimension ref="A1:IP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="250" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="250" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:250" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:250" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1729,7 +1742,7 @@
       <c r="IO2" s="4"/>
       <c r="IP2" s="4"/>
     </row>
-    <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:250" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1743,7 +1756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:250" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -2003,7 +2016,7 @@
       <c r="IO4" s="4"/>
       <c r="IP4" s="4"/>
     </row>
-    <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:250" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
@@ -2263,7 +2276,7 @@
       <c r="IO5" s="4"/>
       <c r="IP5" s="4"/>
     </row>
-    <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:250" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
@@ -2523,7 +2536,7 @@
       <c r="IO6" s="4"/>
       <c r="IP6" s="4"/>
     </row>
-    <row r="7" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:250" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2537,7 +2550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:250" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -2797,7 +2810,7 @@
       <c r="IO8" s="4"/>
       <c r="IP8" s="4"/>
     </row>
-    <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:250" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>34</v>
       </c>
@@ -3057,7 +3070,7 @@
       <c r="IO9" s="4"/>
       <c r="IP9" s="4"/>
     </row>
-    <row r="10" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:250" ht="15" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>33</v>
       </c>
@@ -3317,7 +3330,7 @@
       <c r="IO10" s="4"/>
       <c r="IP10" s="4"/>
     </row>
-    <row r="11" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:250" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3331,7 +3344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:250" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
@@ -3591,7 +3604,7 @@
       <c r="IO12" s="4"/>
       <c r="IP12" s="4"/>
     </row>
-    <row r="13" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:250" ht="15" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
@@ -3851,7 +3864,7 @@
       <c r="IO13" s="4"/>
       <c r="IP13" s="4"/>
     </row>
-    <row r="14" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:250" ht="15" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -4111,7 +4124,7 @@
       <c r="IO14" s="4"/>
       <c r="IP14" s="4"/>
     </row>
-    <row r="15" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:250" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -4125,7 +4138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:250" ht="15" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
@@ -4385,7 +4398,7 @@
       <c r="IO16" s="4"/>
       <c r="IP16" s="4"/>
     </row>
-    <row r="17" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:250" ht="15" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
@@ -4645,7 +4658,7 @@
       <c r="IO17" s="4"/>
       <c r="IP17" s="4"/>
     </row>
-    <row r="18" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:250" ht="15" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>36</v>
       </c>
@@ -4905,7 +4918,7 @@
       <c r="IO18" s="4"/>
       <c r="IP18" s="4"/>
     </row>
-    <row r="19" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:250" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -4919,7 +4932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:250" ht="15" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
@@ -5179,7 +5192,7 @@
       <c r="IO20" s="4"/>
       <c r="IP20" s="4"/>
     </row>
-    <row r="21" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:250" ht="15" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>53</v>
       </c>
@@ -5439,7 +5452,7 @@
       <c r="IO21" s="4"/>
       <c r="IP21" s="4"/>
     </row>
-    <row r="22" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:250" ht="15" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -5699,7 +5712,7 @@
       <c r="IO22" s="4"/>
       <c r="IP22" s="4"/>
     </row>
-    <row r="23" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:250" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -5713,7 +5726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:250" ht="15" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -5973,7 +5986,7 @@
       <c r="IO24" s="4"/>
       <c r="IP24" s="4"/>
     </row>
-    <row r="25" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:250" ht="15" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>51</v>
       </c>
@@ -6233,7 +6246,7 @@
       <c r="IO25" s="4"/>
       <c r="IP25" s="4"/>
     </row>
-    <row r="26" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:250" ht="15" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>52</v>
       </c>
@@ -6247,8 +6260,36 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+    <row r="27" spans="1:250" ht="15" customHeight="1">
+      <c r="A27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:250" ht="15" customHeight="1">
+      <c r="A28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:250" ht="15" customHeight="1">
+      <c r="A30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6265,7 +6306,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: make dure TL is decimal
</commit_message>
<xml_diff>
--- a/dictionaries/methylclocks/mc-yearly-rep.xlsx
+++ b/dictionaries/methylclocks/mc-yearly-rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justiina\Desktop\DNAm age\Methylclock\datashield\ds-beta-dictionaries\dictionaries\methylclocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylclocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E95DCB-2F10-4BA7-811B-54D3901085FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A8BE61-5535-074B-9E28-C831BF2D9CCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="1580" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -199,12 +199,15 @@
   <si>
     <t>Telomere length estimate</t>
   </si>
+  <si>
+    <t>integer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1457,18 +1460,18 @@
   <dimension ref="A1:IP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="250" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="250" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="15" customHeight="1">
+    <row r="1" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:250" ht="15" customHeight="1">
+    <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1745,7 @@
       <c r="IO2" s="4"/>
       <c r="IP2" s="4"/>
     </row>
-    <row r="3" spans="1:250" ht="15" customHeight="1">
+    <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:250" ht="15" customHeight="1">
+    <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -2016,7 +2019,7 @@
       <c r="IO4" s="4"/>
       <c r="IP4" s="4"/>
     </row>
-    <row r="5" spans="1:250" ht="15" customHeight="1">
+    <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="IO5" s="4"/>
       <c r="IP5" s="4"/>
     </row>
-    <row r="6" spans="1:250" ht="15" customHeight="1">
+    <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
@@ -2536,7 +2539,7 @@
       <c r="IO6" s="4"/>
       <c r="IP6" s="4"/>
     </row>
-    <row r="7" spans="1:250" ht="15" customHeight="1">
+    <row r="7" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:250" ht="15" customHeight="1">
+    <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -2810,7 +2813,7 @@
       <c r="IO8" s="4"/>
       <c r="IP8" s="4"/>
     </row>
-    <row r="9" spans="1:250" ht="15" customHeight="1">
+    <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>34</v>
       </c>
@@ -3070,7 +3073,7 @@
       <c r="IO9" s="4"/>
       <c r="IP9" s="4"/>
     </row>
-    <row r="10" spans="1:250" ht="15" customHeight="1">
+    <row r="10" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>33</v>
       </c>
@@ -3330,7 +3333,7 @@
       <c r="IO10" s="4"/>
       <c r="IP10" s="4"/>
     </row>
-    <row r="11" spans="1:250" ht="15" customHeight="1">
+    <row r="11" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:250" ht="15" customHeight="1">
+    <row r="12" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
@@ -3604,7 +3607,7 @@
       <c r="IO12" s="4"/>
       <c r="IP12" s="4"/>
     </row>
-    <row r="13" spans="1:250" ht="15" customHeight="1">
+    <row r="13" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
@@ -3864,7 +3867,7 @@
       <c r="IO13" s="4"/>
       <c r="IP13" s="4"/>
     </row>
-    <row r="14" spans="1:250" ht="15" customHeight="1">
+    <row r="14" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -4124,7 +4127,7 @@
       <c r="IO14" s="4"/>
       <c r="IP14" s="4"/>
     </row>
-    <row r="15" spans="1:250" ht="15" customHeight="1">
+    <row r="15" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:250" ht="15" customHeight="1">
+    <row r="16" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
@@ -4398,7 +4401,7 @@
       <c r="IO16" s="4"/>
       <c r="IP16" s="4"/>
     </row>
-    <row r="17" spans="1:250" ht="15" customHeight="1">
+    <row r="17" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
@@ -4658,7 +4661,7 @@
       <c r="IO17" s="4"/>
       <c r="IP17" s="4"/>
     </row>
-    <row r="18" spans="1:250" ht="15" customHeight="1">
+    <row r="18" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>36</v>
       </c>
@@ -4918,7 +4921,7 @@
       <c r="IO18" s="4"/>
       <c r="IP18" s="4"/>
     </row>
-    <row r="19" spans="1:250" ht="15" customHeight="1">
+    <row r="19" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -4932,7 +4935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:250" ht="15" customHeight="1">
+    <row r="20" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
@@ -5192,7 +5195,7 @@
       <c r="IO20" s="4"/>
       <c r="IP20" s="4"/>
     </row>
-    <row r="21" spans="1:250" ht="15" customHeight="1">
+    <row r="21" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>53</v>
       </c>
@@ -5452,7 +5455,7 @@
       <c r="IO21" s="4"/>
       <c r="IP21" s="4"/>
     </row>
-    <row r="22" spans="1:250" ht="15" customHeight="1">
+    <row r="22" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -5712,7 +5715,7 @@
       <c r="IO22" s="4"/>
       <c r="IP22" s="4"/>
     </row>
-    <row r="23" spans="1:250" ht="15" customHeight="1">
+    <row r="23" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:250" ht="15" customHeight="1">
+    <row r="24" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -5986,7 +5989,7 @@
       <c r="IO24" s="4"/>
       <c r="IP24" s="4"/>
     </row>
-    <row r="25" spans="1:250" ht="15" customHeight="1">
+    <row r="25" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>51</v>
       </c>
@@ -6246,7 +6249,7 @@
       <c r="IO25" s="4"/>
       <c r="IP25" s="4"/>
     </row>
-    <row r="26" spans="1:250" ht="15" customHeight="1">
+    <row r="26" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>52</v>
       </c>
@@ -6260,11 +6263,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:250" ht="15" customHeight="1">
+    <row r="27" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -6274,12 +6277,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:250" ht="15" customHeight="1">
+    <row r="28" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
@@ -6288,7 +6291,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:250" ht="15" customHeight="1">
+    <row r="30" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
   </sheetData>
@@ -6306,7 +6309,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: added additional variables and corrected age
</commit_message>
<xml_diff>
--- a/dictionaries/methylclocks/mc-yearly-rep.xlsx
+++ b/dictionaries/methylclocks/mc-yearly-rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylclocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/RProjects/ds-beta-dictionaries/dictionaries/methylclocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A8BE61-5535-074B-9E28-C831BF2D9CCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A93415B-E62E-004F-B90B-A29319980378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="1580" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -200,29 +200,56 @@
     <t>Telomere length estimate</t>
   </si>
   <si>
-    <t>integer</t>
+    <t>ageAcc.Horvath2</t>
+  </si>
+  <si>
+    <t>ageAcc2.Horvath2</t>
+  </si>
+  <si>
+    <t>ageAcc.TL</t>
+  </si>
+  <si>
+    <t>ageAcc2.TL</t>
+  </si>
+  <si>
+    <t>Age 1 for Horvath 2 measurement</t>
+  </si>
+  <si>
+    <t>Age 2 for Horvath 2 measurement</t>
+  </si>
+  <si>
+    <t>Age 1 for  TL measurement</t>
+  </si>
+  <si>
+    <t>Age 2 for  TL measurement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Arial Unicode MS"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -234,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,11 +295,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -280,11 +335,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1457,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP30"/>
+  <dimension ref="A1:IP32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1763,13 +1820,13 @@
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="4"/>
@@ -2020,16 +2077,16 @@
       <c r="IP4" s="4"/>
     </row>
     <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="4"/>
@@ -2280,16 +2337,16 @@
       <c r="IP5" s="4"/>
     </row>
     <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="4"/>
@@ -2554,16 +2611,16 @@
       </c>
     </row>
     <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="4"/>
@@ -2814,16 +2871,16 @@
       <c r="IP8" s="4"/>
     </row>
     <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E9" s="4"/>
@@ -3074,16 +3131,16 @@
       <c r="IP9" s="4"/>
     </row>
     <row r="10" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="4"/>
@@ -3348,16 +3405,16 @@
       </c>
     </row>
     <row r="12" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="4"/>
@@ -3608,16 +3665,16 @@
       <c r="IP12" s="4"/>
     </row>
     <row r="13" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="4"/>
@@ -3868,16 +3925,16 @@
       <c r="IP13" s="4"/>
     </row>
     <row r="14" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="4"/>
@@ -4142,16 +4199,16 @@
       </c>
     </row>
     <row r="16" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="4"/>
@@ -4402,16 +4459,16 @@
       <c r="IP16" s="4"/>
     </row>
     <row r="17" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="4"/>
@@ -4662,16 +4719,16 @@
       <c r="IP17" s="4"/>
     </row>
     <row r="18" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E18" s="4"/>
@@ -4936,16 +4993,16 @@
       </c>
     </row>
     <row r="20" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="4"/>
@@ -5196,16 +5253,16 @@
       <c r="IP20" s="4"/>
     </row>
     <row r="21" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="4"/>
@@ -5456,16 +5513,16 @@
       <c r="IP21" s="4"/>
     </row>
     <row r="22" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="4"/>
@@ -5730,16 +5787,16 @@
       </c>
     </row>
     <row r="24" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E24" s="4"/>
@@ -5990,16 +6047,16 @@
       <c r="IP24" s="4"/>
     </row>
     <row r="25" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="4"/>
@@ -6250,49 +6307,102 @@
       <c r="IP25" s="4"/>
     </row>
     <row r="26" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>59</v>
+      <c r="B28" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="29" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>